<commit_message>
update testcase and test design
</commit_message>
<xml_diff>
--- a/MiddleAssignment_LeTuanSang/MiddleAssignment_TestDesign1/MiddleAssignment_TestDesign1_LeTuanSang.xlsx
+++ b/MiddleAssignment_LeTuanSang/MiddleAssignment_TestDesign1/MiddleAssignment_TestDesign1_LeTuanSang.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NashTechHomeWork_LeTuanSang\MiddleAssignment\MiddleAssignment_TestDesign1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NashTechHomeWork_LeTuanSang\MiddleAssignment_LeTuanSang\MiddleAssignment_TestDesign1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C9C2B1-32D3-4607-A9AE-0A4B63C8534D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DDB33B-DDF3-420D-8FA7-B93907EF7295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1220,9 +1220,6 @@
     <t>Verify that the big photo frame display only the first photo of photo list which bordered by a red frame. If there is 2 photos on the photo list, the photo left is not framed by a red frame and not displayed on the big photo frame</t>
   </si>
   <si>
-    <t>Verify the integral part of discounted price is displayed if discounted price is decimal and the first numer of decimal part is 5.</t>
-  </si>
-  <si>
     <t>Verify the integral part of discounted price is displayed if discounted price is decimal and the first numer of decimal part is 0.</t>
   </si>
   <si>
@@ -1278,6 +1275,9 @@
   </si>
   <si>
     <t xml:space="preserve">Verify that the big photo frame display nothing if there is no photos on the photo list. </t>
+  </si>
+  <si>
+    <t>Verify the integral part of discounted price is add 1 and displayed if discounted price is decimal and the first numer of decimal part is 5.</t>
   </si>
 </sst>
 </file>
@@ -2960,6 +2960,30 @@
     <xf numFmtId="0" fontId="64" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2975,12 +2999,6 @@
     <xf numFmtId="0" fontId="64" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3038,23 +3056,44 @@
     <xf numFmtId="0" fontId="69" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="18" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="15" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="46" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3062,6 +3101,15 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="43" fillId="12" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -3071,58 +3119,10 @@
     <xf numFmtId="166" fontId="44" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="46" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="18" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="15" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4920,7 +4920,7 @@
   <dimension ref="A1:X101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4935,10 +4935,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="14.25">
-      <c r="A1" s="232"/>
-      <c r="B1" s="232"/>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
+      <c r="A1" s="240"/>
+      <c r="B1" s="240"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
       <c r="E1" s="34"/>
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
@@ -4947,13 +4947,13 @@
       <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" ht="26.25">
-      <c r="A2" s="233" t="s">
+      <c r="A2" s="241" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="233"/>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="259"/>
+      <c r="B2" s="241"/>
+      <c r="C2" s="241"/>
+      <c r="D2" s="241"/>
+      <c r="E2" s="233"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -4963,9 +4963,9 @@
     <row r="3" spans="1:24" s="1" customFormat="1" ht="23.25">
       <c r="A3" s="47"/>
       <c r="B3" s="186"/>
-      <c r="C3" s="260"/>
-      <c r="D3" s="260"/>
-      <c r="E3" s="259"/>
+      <c r="C3" s="234"/>
+      <c r="D3" s="234"/>
+      <c r="E3" s="233"/>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -4992,7 +4992,7 @@
       <c r="A5" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="234"/>
+      <c r="B5" s="236"/>
       <c r="C5" s="235"/>
       <c r="D5" s="235"/>
       <c r="E5" s="39"/>
@@ -5008,7 +5008,7 @@
       <c r="A6" s="132" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="234" t="s">
+      <c r="B6" s="236" t="s">
         <v>199</v>
       </c>
       <c r="C6" s="235"/>
@@ -5039,9 +5039,9 @@
       <c r="A8" s="132" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="236"/>
-      <c r="C8" s="236"/>
-      <c r="D8" s="236"/>
+      <c r="B8" s="242"/>
+      <c r="C8" s="242"/>
+      <c r="D8" s="242"/>
       <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:24" s="43" customFormat="1">
@@ -5184,11 +5184,11 @@
       <c r="C16" s="50"/>
       <c r="D16" s="51"/>
       <c r="E16" s="56"/>
-      <c r="F16" s="255" t="s">
+      <c r="F16" s="229" t="s">
         <v>98</v>
       </c>
-      <c r="G16" s="255"/>
-      <c r="H16" s="255"/>
+      <c r="G16" s="229"/>
+      <c r="H16" s="229"/>
       <c r="I16" s="57"/>
     </row>
     <row r="17" spans="1:9" s="44" customFormat="1">
@@ -5216,11 +5216,11 @@
     </row>
     <row r="18" spans="1:9" s="44" customFormat="1" ht="12.75">
       <c r="A18" s="202"/>
-      <c r="B18" s="256" t="s">
+      <c r="B18" s="230" t="s">
         <v>196</v>
       </c>
-      <c r="C18" s="257"/>
-      <c r="D18" s="258"/>
+      <c r="C18" s="231"/>
+      <c r="D18" s="232"/>
       <c r="E18" s="62"/>
       <c r="F18" s="63"/>
       <c r="G18" s="63"/>
@@ -5229,11 +5229,11 @@
     </row>
     <row r="19" spans="1:9" s="45" customFormat="1">
       <c r="A19" s="52"/>
-      <c r="B19" s="240" t="s">
+      <c r="B19" s="246" t="s">
         <v>205</v>
       </c>
-      <c r="C19" s="241"/>
-      <c r="D19" s="242"/>
+      <c r="C19" s="247"/>
+      <c r="D19" s="248"/>
       <c r="E19" s="180"/>
       <c r="F19" s="181"/>
       <c r="G19" s="181"/>
@@ -5325,7 +5325,7 @@
         <v>6</v>
       </c>
       <c r="B25" s="197" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C25" s="196"/>
       <c r="D25" s="197"/>
@@ -5369,12 +5369,12 @@
     </row>
     <row r="28" spans="1:9" s="45" customFormat="1">
       <c r="A28" s="52"/>
-      <c r="B28" s="252" t="s">
+      <c r="B28" s="258" t="s">
         <v>206</v>
       </c>
-      <c r="C28" s="253"/>
-      <c r="D28" s="253"/>
-      <c r="E28" s="254"/>
+      <c r="C28" s="259"/>
+      <c r="D28" s="259"/>
+      <c r="E28" s="260"/>
       <c r="F28" s="181"/>
       <c r="G28" s="181"/>
       <c r="H28" s="181"/>
@@ -5466,7 +5466,7 @@
         <v>14</v>
       </c>
       <c r="B34" s="199" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C34" s="200"/>
       <c r="D34" s="197"/>
@@ -5510,12 +5510,12 @@
     </row>
     <row r="37" spans="1:10" s="45" customFormat="1">
       <c r="A37" s="52"/>
-      <c r="B37" s="249" t="s">
+      <c r="B37" s="255" t="s">
         <v>207</v>
       </c>
-      <c r="C37" s="250"/>
-      <c r="D37" s="250"/>
-      <c r="E37" s="251"/>
+      <c r="C37" s="256"/>
+      <c r="D37" s="256"/>
+      <c r="E37" s="257"/>
       <c r="F37" s="181"/>
       <c r="G37" s="181"/>
       <c r="H37" s="181"/>
@@ -5527,7 +5527,7 @@
         <v>17</v>
       </c>
       <c r="B38" s="197" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C38" s="196"/>
       <c r="D38" s="197"/>
@@ -5543,7 +5543,7 @@
         <v>18</v>
       </c>
       <c r="B39" s="197" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C39" s="196"/>
       <c r="D39" s="197"/>
@@ -5559,7 +5559,7 @@
         <v>19</v>
       </c>
       <c r="B40" s="197" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C40" s="196"/>
       <c r="D40" s="197"/>
@@ -5575,7 +5575,7 @@
         <v>20</v>
       </c>
       <c r="B41" s="197" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C41" s="196"/>
       <c r="D41" s="197"/>
@@ -5591,7 +5591,7 @@
         <v>21</v>
       </c>
       <c r="B42" s="197" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C42" s="196"/>
       <c r="D42" s="197"/>
@@ -5607,7 +5607,7 @@
         <v>22</v>
       </c>
       <c r="B43" s="185" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C43" s="194"/>
       <c r="D43" s="59"/>
@@ -5623,7 +5623,7 @@
         <v>23</v>
       </c>
       <c r="B44" s="185" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C44" s="159"/>
       <c r="D44" s="60"/>
@@ -5635,11 +5635,11 @@
     </row>
     <row r="45" spans="1:10" s="48" customFormat="1">
       <c r="A45" s="58"/>
-      <c r="B45" s="237" t="s">
+      <c r="B45" s="243" t="s">
         <v>197</v>
       </c>
-      <c r="C45" s="238"/>
-      <c r="D45" s="239"/>
+      <c r="C45" s="244"/>
+      <c r="D45" s="245"/>
       <c r="E45" s="169"/>
       <c r="F45" s="170"/>
       <c r="G45" s="170"/>
@@ -5648,11 +5648,11 @@
     </row>
     <row r="46" spans="1:10" s="178" customFormat="1">
       <c r="A46" s="172"/>
-      <c r="B46" s="243" t="s">
+      <c r="B46" s="249" t="s">
         <v>201</v>
       </c>
-      <c r="C46" s="244"/>
-      <c r="D46" s="245"/>
+      <c r="C46" s="250"/>
+      <c r="D46" s="251"/>
       <c r="E46" s="180"/>
       <c r="F46" s="181"/>
       <c r="G46" s="181"/>
@@ -5697,7 +5697,7 @@
         <v>26</v>
       </c>
       <c r="B49" s="183" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C49" s="174"/>
       <c r="D49" s="174"/>
@@ -5713,7 +5713,7 @@
         <v>27</v>
       </c>
       <c r="B50" s="183" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C50" s="179"/>
       <c r="D50" s="174"/>
@@ -5723,13 +5723,13 @@
       <c r="H50" s="176"/>
       <c r="I50" s="177"/>
     </row>
-    <row r="51" spans="1:9" s="178" customFormat="1" ht="60">
+    <row r="51" spans="1:9" s="178" customFormat="1" ht="75">
       <c r="A51" s="173">
         <f t="shared" ca="1" si="1"/>
         <v>28</v>
       </c>
       <c r="B51" s="183" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="C51" s="201"/>
       <c r="D51" s="174"/>
@@ -5745,7 +5745,7 @@
         <v>29</v>
       </c>
       <c r="B52" s="183" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C52" s="174"/>
       <c r="D52" s="174"/>
@@ -5757,11 +5757,11 @@
     </row>
     <row r="53" spans="1:9" s="49" customFormat="1">
       <c r="A53" s="173"/>
-      <c r="B53" s="246" t="s">
+      <c r="B53" s="252" t="s">
         <v>200</v>
       </c>
-      <c r="C53" s="247"/>
-      <c r="D53" s="248"/>
+      <c r="C53" s="253"/>
+      <c r="D53" s="254"/>
       <c r="E53" s="166"/>
       <c r="F53" s="167"/>
       <c r="G53" s="167"/>
@@ -5774,7 +5774,7 @@
         <v>30</v>
       </c>
       <c r="B54" s="165" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C54" s="164"/>
       <c r="D54" s="164"/>
@@ -5790,7 +5790,7 @@
         <v>31</v>
       </c>
       <c r="B55" s="165" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C55" s="164"/>
       <c r="D55" s="164"/>
@@ -5806,7 +5806,7 @@
         <v>32</v>
       </c>
       <c r="B56" s="165" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C56" s="164"/>
       <c r="D56" s="164"/>
@@ -5822,7 +5822,7 @@
         <v>33</v>
       </c>
       <c r="B57" s="165" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C57" s="164"/>
       <c r="D57" s="164"/>
@@ -5838,7 +5838,7 @@
         <v>34</v>
       </c>
       <c r="B58" s="165" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C58" s="164"/>
       <c r="D58" s="164"/>
@@ -5854,7 +5854,7 @@
         <v>35</v>
       </c>
       <c r="B59" s="165" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C59" s="164"/>
       <c r="D59" s="164"/>
@@ -5870,7 +5870,7 @@
         <v>36</v>
       </c>
       <c r="B60" s="165" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C60" s="164"/>
       <c r="D60" s="164"/>
@@ -6151,9 +6151,9 @@
     </row>
     <row r="85" spans="1:9" s="49" customFormat="1" ht="14.25">
       <c r="A85" s="160"/>
-      <c r="B85" s="229"/>
-      <c r="C85" s="230"/>
-      <c r="D85" s="231"/>
+      <c r="B85" s="237"/>
+      <c r="C85" s="238"/>
+      <c r="D85" s="239"/>
       <c r="E85" s="161"/>
       <c r="F85" s="162"/>
       <c r="G85" s="162"/>
@@ -6195,9 +6195,9 @@
     </row>
     <row r="89" spans="1:9" s="49" customFormat="1" ht="14.25">
       <c r="A89" s="160"/>
-      <c r="B89" s="229"/>
-      <c r="C89" s="230"/>
-      <c r="D89" s="231"/>
+      <c r="B89" s="237"/>
+      <c r="C89" s="238"/>
+      <c r="D89" s="239"/>
       <c r="E89" s="161"/>
       <c r="F89" s="162"/>
       <c r="G89" s="162"/>
@@ -6239,9 +6239,9 @@
     </row>
     <row r="93" spans="1:9" s="49" customFormat="1" ht="14.25">
       <c r="A93" s="160"/>
-      <c r="B93" s="229"/>
-      <c r="C93" s="230"/>
-      <c r="D93" s="231"/>
+      <c r="B93" s="237"/>
+      <c r="C93" s="238"/>
+      <c r="D93" s="239"/>
       <c r="E93" s="161"/>
       <c r="F93" s="162"/>
       <c r="G93" s="162"/>
@@ -6272,9 +6272,9 @@
     </row>
     <row r="96" spans="1:9" s="49" customFormat="1" ht="14.25">
       <c r="A96" s="160"/>
-      <c r="B96" s="229"/>
-      <c r="C96" s="230"/>
-      <c r="D96" s="231"/>
+      <c r="B96" s="237"/>
+      <c r="C96" s="238"/>
+      <c r="D96" s="239"/>
       <c r="E96" s="161"/>
       <c r="F96" s="162"/>
       <c r="G96" s="162"/>
@@ -6338,12 +6338,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
     <mergeCell ref="B89:D89"/>
     <mergeCell ref="B93:D93"/>
     <mergeCell ref="B96:D96"/>
@@ -6359,6 +6353,12 @@
     <mergeCell ref="B53:D53"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
@@ -6415,13 +6415,13 @@
     </row>
     <row r="2" spans="1:12" s="77" customFormat="1" ht="26.25">
       <c r="A2" s="76"/>
-      <c r="C2" s="263" t="s">
+      <c r="C2" s="279" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="263"/>
-      <c r="E2" s="263"/>
-      <c r="F2" s="263"/>
-      <c r="G2" s="263"/>
+      <c r="D2" s="279"/>
+      <c r="E2" s="279"/>
+      <c r="F2" s="279"/>
+      <c r="G2" s="279"/>
       <c r="H2" s="78" t="s">
         <v>112</v>
       </c>
@@ -6432,15 +6432,15 @@
     </row>
     <row r="3" spans="1:12" s="77" customFormat="1" ht="23.25">
       <c r="A3" s="76"/>
-      <c r="C3" s="264" t="s">
+      <c r="C3" s="280" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="264"/>
+      <c r="D3" s="280"/>
       <c r="E3" s="149"/>
-      <c r="F3" s="265" t="s">
+      <c r="F3" s="281" t="s">
         <v>114</v>
       </c>
-      <c r="G3" s="265"/>
+      <c r="G3" s="281"/>
       <c r="H3" s="79"/>
       <c r="I3" s="79"/>
       <c r="J3" s="80"/>
@@ -6465,10 +6465,10 @@
       <c r="L5" s="85"/>
     </row>
     <row r="6" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B6" s="266" t="s">
+      <c r="B6" s="263" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="266"/>
+      <c r="C6" s="263"/>
       <c r="D6" s="87"/>
       <c r="E6" s="87"/>
       <c r="F6" s="87"/>
@@ -6637,11 +6637,11 @@
       <c r="G13" s="91"/>
     </row>
     <row r="14" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B14" s="266" t="s">
+      <c r="B14" s="263" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="266"/>
-      <c r="D14" s="266"/>
+      <c r="C14" s="263"/>
+      <c r="D14" s="263"/>
       <c r="E14" s="87"/>
       <c r="F14" s="87"/>
       <c r="G14" s="88"/>
@@ -6817,11 +6817,11 @@
       <c r="G22" s="91"/>
     </row>
     <row r="23" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B23" s="266" t="s">
+      <c r="B23" s="263" t="s">
         <v>155</v>
       </c>
-      <c r="C23" s="266"/>
-      <c r="D23" s="266"/>
+      <c r="C23" s="263"/>
+      <c r="D23" s="263"/>
       <c r="E23" s="87"/>
       <c r="F23" s="87"/>
       <c r="G23" s="88"/>
@@ -6867,10 +6867,10 @@
       <c r="F26" s="152" t="s">
         <v>162</v>
       </c>
-      <c r="G26" s="267" t="s">
+      <c r="G26" s="282" t="s">
         <v>107</v>
       </c>
-      <c r="H26" s="268"/>
+      <c r="H26" s="283"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="93">
@@ -6895,8 +6895,8 @@
         <f>COUNTIFS(#REF!, "*Critical*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Critical*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G27" s="261"/>
-      <c r="H27" s="262"/>
+      <c r="G27" s="274"/>
+      <c r="H27" s="275"/>
     </row>
     <row r="28" spans="1:12" ht="20.25" customHeight="1">
       <c r="A28" s="93">
@@ -6921,8 +6921,8 @@
         <f>COUNTIFS(#REF!, "*Major*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Major*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G28" s="261"/>
-      <c r="H28" s="262"/>
+      <c r="G28" s="274"/>
+      <c r="H28" s="275"/>
     </row>
     <row r="29" spans="1:12" ht="20.25" customHeight="1">
       <c r="A29" s="93">
@@ -6947,8 +6947,8 @@
         <f>COUNTIFS(#REF!, "*Normal*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Normal*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G29" s="261"/>
-      <c r="H29" s="262"/>
+      <c r="G29" s="274"/>
+      <c r="H29" s="275"/>
     </row>
     <row r="30" spans="1:12" ht="20.25" customHeight="1">
       <c r="A30" s="93">
@@ -6973,8 +6973,8 @@
         <f>COUNTIFS(#REF!, "*Minor*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Minor*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G30" s="261"/>
-      <c r="H30" s="262"/>
+      <c r="G30" s="274"/>
+      <c r="H30" s="275"/>
     </row>
     <row r="31" spans="1:12" ht="20.25" customHeight="1">
       <c r="A31" s="93"/>
@@ -6995,8 +6995,8 @@
         <f>SUM(F27:F30)</f>
         <v>#REF!</v>
       </c>
-      <c r="G31" s="261"/>
-      <c r="H31" s="262"/>
+      <c r="G31" s="274"/>
+      <c r="H31" s="275"/>
     </row>
     <row r="32" spans="1:12" ht="20.25" customHeight="1">
       <c r="A32" s="99"/>
@@ -7034,7 +7034,7 @@
       <c r="E34" s="152" t="s">
         <v>121</v>
       </c>
-      <c r="F34" s="269" t="s">
+      <c r="F34" s="268" t="s">
         <v>124</v>
       </c>
       <c r="G34" s="270"/>
@@ -7053,8 +7053,8 @@
       <c r="E35" s="119" t="s">
         <v>129</v>
       </c>
-      <c r="F35" s="272"/>
-      <c r="G35" s="273"/>
+      <c r="F35" s="277"/>
+      <c r="G35" s="278"/>
       <c r="H35" s="117"/>
       <c r="I35" s="117"/>
       <c r="J35" s="117"/>
@@ -7077,8 +7077,8 @@
       <c r="E36" s="97" t="s">
         <v>135</v>
       </c>
-      <c r="F36" s="261"/>
-      <c r="G36" s="262"/>
+      <c r="F36" s="274"/>
+      <c r="G36" s="275"/>
     </row>
     <row r="37" spans="1:12" ht="20.25" customHeight="1">
       <c r="A37" s="93">
@@ -7096,8 +7096,8 @@
       <c r="E37" s="97" t="s">
         <v>135</v>
       </c>
-      <c r="F37" s="261"/>
-      <c r="G37" s="262"/>
+      <c r="F37" s="274"/>
+      <c r="G37" s="275"/>
     </row>
     <row r="38" spans="1:12" ht="20.25" customHeight="1">
       <c r="A38" s="99"/>
@@ -7110,10 +7110,10 @@
       <c r="H38" s="101"/>
     </row>
     <row r="39" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B39" s="266" t="s">
+      <c r="B39" s="263" t="s">
         <v>176</v>
       </c>
-      <c r="C39" s="266"/>
+      <c r="C39" s="263"/>
       <c r="D39" s="87"/>
       <c r="E39" s="87"/>
       <c r="F39" s="87"/>
@@ -7137,15 +7137,15 @@
       <c r="B41" s="152" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="271" t="s">
+      <c r="C41" s="276" t="s">
         <v>178</v>
       </c>
-      <c r="D41" s="271"/>
-      <c r="E41" s="271" t="s">
+      <c r="D41" s="276"/>
+      <c r="E41" s="276" t="s">
         <v>179</v>
       </c>
-      <c r="F41" s="271"/>
-      <c r="G41" s="271"/>
+      <c r="F41" s="276"/>
+      <c r="G41" s="276"/>
       <c r="H41" s="92" t="s">
         <v>180</v>
       </c>
@@ -7157,15 +7157,15 @@
       <c r="B42" s="153" t="s">
         <v>181</v>
       </c>
-      <c r="C42" s="274" t="s">
+      <c r="C42" s="273" t="s">
         <v>182</v>
       </c>
-      <c r="D42" s="274"/>
-      <c r="E42" s="274" t="s">
+      <c r="D42" s="273"/>
+      <c r="E42" s="273" t="s">
         <v>183</v>
       </c>
-      <c r="F42" s="274"/>
-      <c r="G42" s="274"/>
+      <c r="F42" s="273"/>
+      <c r="G42" s="273"/>
       <c r="H42" s="102"/>
     </row>
     <row r="43" spans="1:12" ht="34.5" customHeight="1">
@@ -7175,15 +7175,15 @@
       <c r="B43" s="153" t="s">
         <v>181</v>
       </c>
-      <c r="C43" s="274" t="s">
+      <c r="C43" s="273" t="s">
         <v>182</v>
       </c>
-      <c r="D43" s="274"/>
-      <c r="E43" s="274" t="s">
+      <c r="D43" s="273"/>
+      <c r="E43" s="273" t="s">
         <v>183</v>
       </c>
-      <c r="F43" s="274"/>
-      <c r="G43" s="274"/>
+      <c r="F43" s="273"/>
+      <c r="G43" s="273"/>
       <c r="H43" s="102"/>
     </row>
     <row r="44" spans="1:12" ht="34.5" customHeight="1">
@@ -7193,15 +7193,15 @@
       <c r="B44" s="153" t="s">
         <v>181</v>
       </c>
-      <c r="C44" s="274" t="s">
+      <c r="C44" s="273" t="s">
         <v>182</v>
       </c>
-      <c r="D44" s="274"/>
-      <c r="E44" s="274" t="s">
+      <c r="D44" s="273"/>
+      <c r="E44" s="273" t="s">
         <v>183</v>
       </c>
-      <c r="F44" s="274"/>
-      <c r="G44" s="274"/>
+      <c r="F44" s="273"/>
+      <c r="G44" s="273"/>
       <c r="H44" s="102"/>
     </row>
     <row r="45" spans="1:12">
@@ -7213,10 +7213,10 @@
       <c r="G45" s="91"/>
     </row>
     <row r="46" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B46" s="266" t="s">
+      <c r="B46" s="263" t="s">
         <v>184</v>
       </c>
-      <c r="C46" s="266"/>
+      <c r="C46" s="263"/>
       <c r="D46" s="87"/>
       <c r="E46" s="87"/>
       <c r="F46" s="87"/>
@@ -7234,25 +7234,25 @@
       <c r="G47" s="91"/>
     </row>
     <row r="48" spans="1:12" s="106" customFormat="1" ht="21" customHeight="1">
-      <c r="A48" s="277" t="s">
+      <c r="A48" s="264" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="279" t="s">
+      <c r="B48" s="266" t="s">
         <v>186</v>
       </c>
-      <c r="C48" s="269" t="s">
+      <c r="C48" s="268" t="s">
         <v>187</v>
       </c>
-      <c r="D48" s="281"/>
-      <c r="E48" s="281"/>
+      <c r="D48" s="269"/>
+      <c r="E48" s="269"/>
       <c r="F48" s="270"/>
-      <c r="G48" s="282" t="s">
+      <c r="G48" s="271" t="s">
         <v>154</v>
       </c>
-      <c r="H48" s="282" t="s">
+      <c r="H48" s="271" t="s">
         <v>186</v>
       </c>
-      <c r="I48" s="275" t="s">
+      <c r="I48" s="261" t="s">
         <v>188</v>
       </c>
       <c r="J48" s="105"/>
@@ -7260,8 +7260,8 @@
       <c r="L48" s="105"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="278"/>
-      <c r="B49" s="280"/>
+      <c r="A49" s="265"/>
+      <c r="B49" s="267"/>
       <c r="C49" s="107" t="s">
         <v>163</v>
       </c>
@@ -7274,13 +7274,13 @@
       <c r="F49" s="108" t="s">
         <v>166</v>
       </c>
-      <c r="G49" s="283"/>
-      <c r="H49" s="283"/>
-      <c r="I49" s="276"/>
+      <c r="G49" s="272"/>
+      <c r="H49" s="272"/>
+      <c r="I49" s="262"/>
     </row>
     <row r="50" spans="1:9" ht="38.25">
-      <c r="A50" s="278"/>
-      <c r="B50" s="280"/>
+      <c r="A50" s="265"/>
+      <c r="B50" s="267"/>
       <c r="C50" s="121" t="s">
         <v>189</v>
       </c>
@@ -7392,26 +7392,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="F35:G35"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C3:D3"/>
@@ -7424,6 +7404,26 @@
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G30:H30"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:H49"/>
   </mergeCells>
   <conditionalFormatting sqref="H51">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
@@ -7461,6 +7461,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008DD9373D9A24F64F89F14F461305A106" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="edefd2bea9a69e65a3918d4b9d850884">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cabca498-5e2a-459c-ade0-601c6a98c846" xmlns:ns3="044e8ed5-b60c-40cd-b477-04c240ccf9c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1cdcf90a8e7cb27405451b504492cec2" ns2:_="" ns3:_="">
     <xsd:import namespace="cabca498-5e2a-459c-ade0-601c6a98c846"/>
@@ -7625,22 +7640,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E3E4FA-795A-4742-A021-9CDC3210C50B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F8C6C6D-E626-49D4-9BA8-E27B2B9C9191}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7729ACD-7A20-4344-BFA5-B224A8419F45}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7657,21 +7674,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F8C6C6D-E626-49D4-9BA8-E27B2B9C9191}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E3E4FA-795A-4742-A021-9CDC3210C50B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>